<commit_message>
Minor edits to Excel charts
</commit_message>
<xml_diff>
--- a/memaccess/charts.xlsx
+++ b/memaccess/charts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andy/clj/jafingerhut.github.com/memaccess/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13AE8959-0F4C-5F49-9F05-8FA9959B1770}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2FF3438-F7FD-AE46-9FE7-47201B33F5B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1620" yWindow="760" windowWidth="32940" windowHeight="21580" activeTab="4" xr2:uid="{081F3700-75E8-5441-97C6-4D48A715C7EA}"/>
+    <workbookView xWindow="1620" yWindow="760" windowWidth="32940" windowHeight="21580" xr2:uid="{081F3700-75E8-5441-97C6-4D48A715C7EA}"/>
   </bookViews>
   <sheets>
     <sheet name="2023 M2 Pro" sheetId="1" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="20">
   <si>
     <t>size_bytes</t>
   </si>
@@ -81,13 +81,41 @@
   <si>
     <t>NEGATIVE STRIDES</t>
   </si>
+  <si>
+    <t>Clock speed (GHz)</t>
+  </si>
+  <si>
+    <t>clock period (nsec)</t>
+  </si>
+  <si>
+    <t>clock cycles</t>
+  </si>
+  <si>
+    <t>512 KB on-chip cache</t>
+  </si>
+  <si>
+    <t>64 KB L1 cache</t>
+  </si>
+  <si>
+    <t>6 MB shared L3 cache</t>
+  </si>
+  <si>
+    <t>~6 adds per 3.7GHz clock period</t>
+  </si>
+  <si>
+    <t>256 KB L2 cache</t>
+  </si>
+  <si>
+    <t>3 MB L3 cache</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -118,11 +146,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11886,6 +11916,7 @@
           <c:logBase val="2"/>
           <c:orientation val="minMax"/>
           <c:max val="5.12"/>
+          <c:min val="0.01"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -14218,37 +14249,37 @@
                 <c:pt idx="9">
                   <c:v>2.5366E-2</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="10">
                   <c:v>2.5017000000000001E-2</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="11">
                   <c:v>2.5201999999999999E-2</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="General">
+                <c:pt idx="12">
                   <c:v>2.6096999999999999E-2</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="General">
+                <c:pt idx="13">
                   <c:v>3.4433999999999999E-2</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="General">
+                <c:pt idx="14">
                   <c:v>4.7648000000000003E-2</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="General">
+                <c:pt idx="15">
                   <c:v>5.3926000000000002E-2</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="General">
+                <c:pt idx="16">
                   <c:v>5.6356000000000003E-2</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="General">
+                <c:pt idx="17">
                   <c:v>7.0610000000000006E-2</c:v>
                 </c:pt>
-                <c:pt idx="18" formatCode="General">
+                <c:pt idx="18">
                   <c:v>7.3663999999999993E-2</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="General">
+                <c:pt idx="19">
                   <c:v>7.2221999999999995E-2</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="General">
+                <c:pt idx="20">
                   <c:v>7.0574999999999999E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -14407,37 +14438,37 @@
                 <c:pt idx="9">
                   <c:v>0.117046</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="10">
                   <c:v>0.116799</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="11">
                   <c:v>0.121452</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="General">
+                <c:pt idx="12">
                   <c:v>0.13021199999999999</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="General">
+                <c:pt idx="13">
                   <c:v>0.16921800000000001</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="General">
+                <c:pt idx="14">
                   <c:v>0.206788</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="General">
+                <c:pt idx="15">
                   <c:v>0.21967999999999999</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="General">
+                <c:pt idx="16">
                   <c:v>0.22332399999999999</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="General">
+                <c:pt idx="17">
                   <c:v>0.25789400000000001</c:v>
                 </c:pt>
-                <c:pt idx="18" formatCode="General">
+                <c:pt idx="18">
                   <c:v>0.30150300000000002</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="General">
+                <c:pt idx="19">
                   <c:v>0.301344</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="General">
+                <c:pt idx="20">
                   <c:v>0.296462</c:v>
                 </c:pt>
               </c:numCache>
@@ -14596,37 +14627,37 @@
                 <c:pt idx="9">
                   <c:v>0.359292</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="10">
                   <c:v>0.361761</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="11">
                   <c:v>0.36088799999999999</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="General">
+                <c:pt idx="12">
                   <c:v>0.38137100000000002</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="General">
+                <c:pt idx="13">
                   <c:v>0.51552699999999996</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="General">
+                <c:pt idx="14">
                   <c:v>0.71517500000000001</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="General">
+                <c:pt idx="15">
                   <c:v>0.77917800000000004</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="General">
+                <c:pt idx="16">
                   <c:v>0.81923800000000002</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="General">
+                <c:pt idx="17">
                   <c:v>0.90912999999999999</c:v>
                 </c:pt>
-                <c:pt idx="18" formatCode="General">
+                <c:pt idx="18">
                   <c:v>1.101567</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="General">
+                <c:pt idx="19">
                   <c:v>1.251044</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="General">
+                <c:pt idx="20">
                   <c:v>1.1014969999999999</c:v>
                 </c:pt>
               </c:numCache>
@@ -14785,37 +14816,37 @@
                 <c:pt idx="9">
                   <c:v>0.41991099999999998</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="10">
                   <c:v>0.43349799999999999</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="11">
                   <c:v>0.42451100000000003</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="General">
+                <c:pt idx="12">
                   <c:v>0.46498</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="General">
+                <c:pt idx="13">
                   <c:v>0.72057400000000005</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="General">
+                <c:pt idx="14">
                   <c:v>0.968669</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="General">
+                <c:pt idx="15">
                   <c:v>1.1142559999999999</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="General">
+                <c:pt idx="16">
                   <c:v>1.1763300000000001</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="General">
+                <c:pt idx="17">
                   <c:v>1.29175</c:v>
                 </c:pt>
-                <c:pt idx="18" formatCode="General">
+                <c:pt idx="18">
                   <c:v>1.634468</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="General">
+                <c:pt idx="19">
                   <c:v>1.6606959999999999</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="General">
+                <c:pt idx="20">
                   <c:v>1.633999</c:v>
                 </c:pt>
               </c:numCache>
@@ -14974,37 +15005,37 @@
                 <c:pt idx="9">
                   <c:v>0.44120399999999999</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="10">
                   <c:v>0.43933899999999998</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="11">
                   <c:v>0.451376</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="General">
+                <c:pt idx="12">
                   <c:v>0.49726500000000001</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="General">
+                <c:pt idx="13">
                   <c:v>0.73631000000000002</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="General">
+                <c:pt idx="14">
                   <c:v>1.0328809999999999</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="General">
+                <c:pt idx="15">
                   <c:v>1.2128270000000001</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="General">
+                <c:pt idx="16">
                   <c:v>1.2693030000000001</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="General">
+                <c:pt idx="17">
                   <c:v>1.4200440000000001</c:v>
                 </c:pt>
-                <c:pt idx="18" formatCode="General">
+                <c:pt idx="18">
                   <c:v>1.736029</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="General">
+                <c:pt idx="19">
                   <c:v>1.9342950000000001</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="General">
+                <c:pt idx="20">
                   <c:v>1.971106</c:v>
                 </c:pt>
               </c:numCache>
@@ -15169,37 +15200,37 @@
                 <c:pt idx="9">
                   <c:v>0.37690800000000002</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="10">
                   <c:v>0.38187399999999999</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="11">
                   <c:v>0.38589000000000001</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="General">
+                <c:pt idx="12">
                   <c:v>0.44257999999999997</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="General">
+                <c:pt idx="13">
                   <c:v>0.65790899999999997</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="General">
+                <c:pt idx="14">
                   <c:v>0.95035599999999998</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="General">
+                <c:pt idx="15">
                   <c:v>1.0979890000000001</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="General">
+                <c:pt idx="16">
                   <c:v>1.157942</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="General">
+                <c:pt idx="17">
                   <c:v>1.3849089999999999</c:v>
                 </c:pt>
-                <c:pt idx="18" formatCode="General">
+                <c:pt idx="18">
                   <c:v>1.724348</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="General">
+                <c:pt idx="19">
                   <c:v>1.819809</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="General">
+                <c:pt idx="20">
                   <c:v>1.803272</c:v>
                 </c:pt>
               </c:numCache>
@@ -15364,37 +15395,37 @@
                 <c:pt idx="9">
                   <c:v>0.37658599999999998</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="10">
                   <c:v>0.383658</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="11">
                   <c:v>0.37719999999999998</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="General">
+                <c:pt idx="12">
                   <c:v>0.46590199999999998</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="General">
+                <c:pt idx="13">
                   <c:v>0.68644700000000003</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="General">
+                <c:pt idx="14">
                   <c:v>0.92892600000000003</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="General">
+                <c:pt idx="15">
                   <c:v>1.107888</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="General">
+                <c:pt idx="16">
                   <c:v>1.1636679999999999</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="General">
+                <c:pt idx="17">
                   <c:v>1.396841</c:v>
                 </c:pt>
-                <c:pt idx="18" formatCode="General">
+                <c:pt idx="18">
                   <c:v>1.914712</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="General">
+                <c:pt idx="19">
                   <c:v>1.920974</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="General">
+                <c:pt idx="20">
                   <c:v>1.9602550000000001</c:v>
                 </c:pt>
               </c:numCache>
@@ -15527,7 +15558,7 @@
             <c:numRef>
               <c:f>'2014 MacBookPro'!$K$14:$K$35</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -15722,7 +15753,7 @@
             <c:numRef>
               <c:f>'2014 MacBookPro'!$L$14:$L$35</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -16209,37 +16240,37 @@
                 <c:pt idx="9">
                   <c:v>0.13526199999999999</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="10">
                   <c:v>0.13214400000000001</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="11">
                   <c:v>0.13305600000000001</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="General">
+                <c:pt idx="12">
                   <c:v>0.14038100000000001</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="General">
+                <c:pt idx="13">
                   <c:v>0.13646800000000001</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="General">
+                <c:pt idx="14">
                   <c:v>0.14415</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="General">
+                <c:pt idx="15">
                   <c:v>0.14243</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="General">
+                <c:pt idx="16">
                   <c:v>0.144763</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="General">
+                <c:pt idx="17">
                   <c:v>0.14199999999999999</c:v>
                 </c:pt>
-                <c:pt idx="18" formatCode="General">
+                <c:pt idx="18">
                   <c:v>0.15577099999999999</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="General">
+                <c:pt idx="19">
                   <c:v>0.152559</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="General">
+                <c:pt idx="20">
                   <c:v>0.149529</c:v>
                 </c:pt>
               </c:numCache>
@@ -16398,37 +16429,37 @@
                 <c:pt idx="9">
                   <c:v>0.140957</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="10">
                   <c:v>0.140038</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="11">
                   <c:v>0.141737</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="General">
+                <c:pt idx="12">
                   <c:v>0.157697</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="General">
+                <c:pt idx="13">
                   <c:v>0.17319899999999999</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="General">
+                <c:pt idx="14">
                   <c:v>0.20987900000000001</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="General">
+                <c:pt idx="15">
                   <c:v>0.22158700000000001</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="General">
+                <c:pt idx="16">
                   <c:v>0.227932</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="General">
+                <c:pt idx="17">
                   <c:v>0.26524999999999999</c:v>
                 </c:pt>
-                <c:pt idx="18" formatCode="General">
+                <c:pt idx="18">
                   <c:v>0.30995200000000001</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="General">
+                <c:pt idx="19">
                   <c:v>0.30471199999999998</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="General">
+                <c:pt idx="20">
                   <c:v>0.29759099999999999</c:v>
                 </c:pt>
               </c:numCache>
@@ -16587,37 +16618,37 @@
                 <c:pt idx="9">
                   <c:v>0.36049100000000001</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="10">
                   <c:v>0.35921199999999998</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="11">
                   <c:v>0.35838300000000001</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="General">
+                <c:pt idx="12">
                   <c:v>0.37626100000000001</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="General">
+                <c:pt idx="13">
                   <c:v>0.50101499999999999</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="General">
+                <c:pt idx="14">
                   <c:v>0.70927200000000001</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="General">
+                <c:pt idx="15">
                   <c:v>0.78307199999999999</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="General">
+                <c:pt idx="16">
                   <c:v>0.804257</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="General">
+                <c:pt idx="17">
                   <c:v>0.91329700000000003</c:v>
                 </c:pt>
-                <c:pt idx="18" formatCode="General">
+                <c:pt idx="18">
                   <c:v>1.1263840000000001</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="General">
+                <c:pt idx="19">
                   <c:v>1.0934269999999999</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="General">
+                <c:pt idx="20">
                   <c:v>1.127624</c:v>
                 </c:pt>
               </c:numCache>
@@ -16776,37 +16807,37 @@
                 <c:pt idx="9">
                   <c:v>0.42336499999999999</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="10">
                   <c:v>0.42436499999999999</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="11">
                   <c:v>0.42604900000000001</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="General">
+                <c:pt idx="12">
                   <c:v>0.45872400000000002</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="General">
+                <c:pt idx="13">
                   <c:v>0.66889600000000005</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="General">
+                <c:pt idx="14">
                   <c:v>0.93852599999999997</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="General">
+                <c:pt idx="15">
                   <c:v>1.0883020000000001</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="General">
+                <c:pt idx="16">
                   <c:v>1.1450819999999999</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="General">
+                <c:pt idx="17">
                   <c:v>1.2915989999999999</c:v>
                 </c:pt>
-                <c:pt idx="18" formatCode="General">
+                <c:pt idx="18">
                   <c:v>1.6532230000000001</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="General">
+                <c:pt idx="19">
                   <c:v>1.5983719999999999</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="General">
+                <c:pt idx="20">
                   <c:v>1.6495610000000001</c:v>
                 </c:pt>
               </c:numCache>
@@ -16965,37 +16996,37 @@
                 <c:pt idx="9">
                   <c:v>0.43804399999999999</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="10">
                   <c:v>0.434498</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="11">
                   <c:v>0.44006400000000001</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="General">
+                <c:pt idx="12">
                   <c:v>0.49197999999999997</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="General">
+                <c:pt idx="13">
                   <c:v>0.73406899999999997</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="General">
+                <c:pt idx="14">
                   <c:v>1.0193099999999999</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="General">
+                <c:pt idx="15">
                   <c:v>1.2228429999999999</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="General">
+                <c:pt idx="16">
                   <c:v>1.2818849999999999</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="General">
+                <c:pt idx="17">
                   <c:v>1.41615</c:v>
                 </c:pt>
-                <c:pt idx="18" formatCode="General">
+                <c:pt idx="18">
                   <c:v>1.6704969999999999</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="General">
+                <c:pt idx="19">
                   <c:v>1.9011640000000001</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="General">
+                <c:pt idx="20">
                   <c:v>1.997838</c:v>
                 </c:pt>
               </c:numCache>
@@ -17160,37 +17191,37 @@
                 <c:pt idx="9">
                   <c:v>0.37545600000000001</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="10">
                   <c:v>0.377216</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="11">
                   <c:v>0.38098599999999999</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="General">
+                <c:pt idx="12">
                   <c:v>0.44505899999999998</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="General">
+                <c:pt idx="13">
                   <c:v>0.657744</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="General">
+                <c:pt idx="14">
                   <c:v>0.92188499999999995</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="General">
+                <c:pt idx="15">
                   <c:v>1.0821419999999999</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="General">
+                <c:pt idx="16">
                   <c:v>1.1663239999999999</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="General">
+                <c:pt idx="17">
                   <c:v>1.3512980000000001</c:v>
                 </c:pt>
-                <c:pt idx="18" formatCode="General">
+                <c:pt idx="18">
                   <c:v>1.604136</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="General">
+                <c:pt idx="19">
                   <c:v>1.794411</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="General">
+                <c:pt idx="20">
                   <c:v>1.8553649999999999</c:v>
                 </c:pt>
               </c:numCache>
@@ -17355,37 +17386,37 @@
                 <c:pt idx="9">
                   <c:v>0.379187</c:v>
                 </c:pt>
-                <c:pt idx="10" formatCode="General">
+                <c:pt idx="10">
                   <c:v>0.377438</c:v>
                 </c:pt>
-                <c:pt idx="11" formatCode="General">
+                <c:pt idx="11">
                   <c:v>0.380019</c:v>
                 </c:pt>
-                <c:pt idx="12" formatCode="General">
+                <c:pt idx="12">
                   <c:v>0.48186499999999999</c:v>
                 </c:pt>
-                <c:pt idx="13" formatCode="General">
+                <c:pt idx="13">
                   <c:v>0.66620100000000004</c:v>
                 </c:pt>
-                <c:pt idx="14" formatCode="General">
+                <c:pt idx="14">
                   <c:v>0.91894500000000001</c:v>
                 </c:pt>
-                <c:pt idx="15" formatCode="General">
+                <c:pt idx="15">
                   <c:v>1.109518</c:v>
                 </c:pt>
-                <c:pt idx="16" formatCode="General">
+                <c:pt idx="16">
                   <c:v>1.1638470000000001</c:v>
                 </c:pt>
-                <c:pt idx="17" formatCode="General">
+                <c:pt idx="17">
                   <c:v>1.403705</c:v>
                 </c:pt>
-                <c:pt idx="18" formatCode="General">
+                <c:pt idx="18">
                   <c:v>1.729077</c:v>
                 </c:pt>
-                <c:pt idx="19" formatCode="General">
+                <c:pt idx="19">
                   <c:v>1.9121269999999999</c:v>
                 </c:pt>
-                <c:pt idx="20" formatCode="General">
+                <c:pt idx="20">
                   <c:v>1.9874510000000001</c:v>
                 </c:pt>
               </c:numCache>
@@ -17518,7 +17549,7 @@
             <c:numRef>
               <c:f>'2014 MacBookPro'!$W$14:$W$35</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -17713,7 +17744,7 @@
             <c:numRef>
               <c:f>'2014 MacBookPro'!$X$14:$X$35</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
@@ -26073,7 +26104,7 @@
   </sheetPr>
   <dimension ref="C1:X34"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B36" sqref="B36:X76"/>
     </sheetView>
   </sheetViews>
@@ -29105,10 +29136,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="C1:X34"/>
+  <dimension ref="B1:X34"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:X76"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -29159,16 +29190,15 @@
     </row>
     <row r="7" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C7" s="3">
-        <f>0.01</f>
-        <v>0.01</v>
+        <v>1.6E-2</v>
       </c>
       <c r="D7" s="1">
         <f>2^28/C7</f>
-        <v>26843545600</v>
+        <v>16777216000</v>
       </c>
       <c r="E7" s="2">
         <f>10^9/D7</f>
-        <v>3.7252902984619141E-2</v>
+        <v>5.9604644775390625E-2</v>
       </c>
       <c r="O7" s="3"/>
       <c r="P7" s="1"/>
@@ -29176,15 +29206,15 @@
     </row>
     <row r="8" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C8" s="3">
-        <v>0.1</v>
+        <v>0.16</v>
       </c>
       <c r="D8" s="1">
         <f>2^28/C8</f>
-        <v>2684354560</v>
+        <v>1677721600</v>
       </c>
       <c r="E8" s="2">
         <f>10^9/D8</f>
-        <v>0.37252902984619141</v>
+        <v>0.59604644775390625</v>
       </c>
       <c r="O8" s="3"/>
       <c r="P8" s="1"/>
@@ -29208,15 +29238,15 @@
     </row>
     <row r="10" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C10" s="3">
-        <v>3</v>
+        <v>1.7</v>
       </c>
       <c r="D10" s="1">
         <f>2^28/C10</f>
-        <v>89478485.333333328</v>
+        <v>157903209.41176471</v>
       </c>
       <c r="E10" s="2">
         <f>10^9/D10</f>
-        <v>11.175870895385742</v>
+        <v>6.3329935073852539</v>
       </c>
       <c r="O10" s="3"/>
       <c r="P10" s="1"/>
@@ -29224,15 +29254,15 @@
     </row>
     <row r="11" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C11" s="3">
-        <v>5</v>
+        <v>3.4</v>
       </c>
       <c r="D11" s="1">
         <f>2^28/C11</f>
-        <v>53687091.200000003</v>
+        <v>78951604.705882356</v>
       </c>
       <c r="E11" s="2">
         <f>10^9/D11</f>
-        <v>18.62645149230957</v>
+        <v>12.665987014770508</v>
       </c>
       <c r="O11" s="3"/>
       <c r="P11" s="1"/>
@@ -29494,7 +29524,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C17" s="1">
         <v>8192</v>
       </c>
@@ -29556,7 +29586,7 @@
         <v>0.19716700000000001</v>
       </c>
     </row>
-    <row r="18" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C18" s="1">
         <v>16384</v>
       </c>
@@ -29618,7 +29648,7 @@
         <v>0.20296</v>
       </c>
     </row>
-    <row r="19" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C19" s="1">
         <v>32768</v>
       </c>
@@ -29680,7 +29710,7 @@
         <v>0.170769</v>
       </c>
     </row>
-    <row r="20" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C20" s="1">
         <v>65536</v>
       </c>
@@ -29742,7 +29772,7 @@
         <v>0.17030699999999999</v>
       </c>
     </row>
-    <row r="21" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C21" s="1">
         <v>131072</v>
       </c>
@@ -29804,7 +29834,10 @@
         <v>0.28419800000000001</v>
       </c>
     </row>
-    <row r="22" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B22" t="s">
+        <v>18</v>
+      </c>
       <c r="C22" s="1">
         <v>262144</v>
       </c>
@@ -29866,7 +29899,7 @@
         <v>0.41384900000000002</v>
       </c>
     </row>
-    <row r="23" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C23" s="1">
         <v>524288</v>
       </c>
@@ -29928,7 +29961,7 @@
         <v>0.51241099999999995</v>
       </c>
     </row>
-    <row r="24" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C24" s="1">
         <v>1048576</v>
       </c>
@@ -29990,7 +30023,7 @@
         <v>0.51654199999999995</v>
       </c>
     </row>
-    <row r="25" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C25" s="1">
         <v>2097152</v>
       </c>
@@ -30052,7 +30085,10 @@
         <v>0.73488500000000001</v>
       </c>
     </row>
-    <row r="26" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
       <c r="C26" s="1">
         <v>4194304</v>
       </c>
@@ -30114,7 +30150,7 @@
         <v>1.418882</v>
       </c>
     </row>
-    <row r="27" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C27" s="1">
         <v>8388608</v>
       </c>
@@ -30176,7 +30212,7 @@
         <v>2.6723870000000001</v>
       </c>
     </row>
-    <row r="28" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C28" s="1">
         <v>16777216</v>
       </c>
@@ -30238,7 +30274,7 @@
         <v>3.0394079999999999</v>
       </c>
     </row>
-    <row r="29" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C29" s="1">
         <v>33554432</v>
       </c>
@@ -30300,7 +30336,7 @@
         <v>3.2709519999999999</v>
       </c>
     </row>
-    <row r="30" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C30" s="1">
         <v>67108864</v>
       </c>
@@ -30362,7 +30398,7 @@
         <v>2.9156939999999998</v>
       </c>
     </row>
-    <row r="31" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C31" s="1">
         <v>134217728</v>
       </c>
@@ -30424,7 +30460,7 @@
         <v>3.0132020000000002</v>
       </c>
     </row>
-    <row r="32" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C32" s="1">
         <v>268435456</v>
       </c>
@@ -30622,10 +30658,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="C1:X34"/>
+  <dimension ref="B1:X35"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:X76"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -30676,16 +30712,24 @@
     </row>
     <row r="7" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C7" s="3">
-        <f>0.01</f>
-        <v>0.01</v>
+        <v>1.2E-2</v>
       </c>
       <c r="D7" s="1">
         <f>2^28/C7</f>
-        <v>26843545600</v>
+        <v>22369621333.333332</v>
       </c>
       <c r="E7" s="2">
         <f>10^9/D7</f>
-        <v>3.7252902984619141E-2</v>
+        <v>4.4703483581542969E-2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
+        <v>12</v>
       </c>
       <c r="O7" s="3"/>
       <c r="P7" s="1"/>
@@ -30693,15 +30737,22 @@
     </row>
     <row r="8" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C8" s="3">
-        <v>0.1</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="D8" s="1">
         <f>2^28/C8</f>
-        <v>2684354560</v>
+        <v>1988410785.185185</v>
       </c>
       <c r="E8" s="2">
         <f>10^9/D8</f>
-        <v>0.37252902984619141</v>
+        <v>0.50291419029235851</v>
+      </c>
+      <c r="H8">
+        <v>2.5</v>
+      </c>
+      <c r="I8" s="4">
+        <f>1/H8</f>
+        <v>0.4</v>
       </c>
       <c r="O8" s="3"/>
       <c r="P8" s="1"/>
@@ -30709,15 +30760,22 @@
     </row>
     <row r="9" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C9" s="3">
-        <v>1</v>
+        <v>0.4</v>
       </c>
       <c r="D9" s="1">
         <f>2^28/C9</f>
-        <v>268435456</v>
+        <v>671088640</v>
       </c>
       <c r="E9" s="2">
         <f>10^9/D9</f>
-        <v>3.7252902984619141</v>
+        <v>1.4901161193847656</v>
+      </c>
+      <c r="H9">
+        <v>3.7</v>
+      </c>
+      <c r="I9" s="4">
+        <f>1/H9</f>
+        <v>0.27027027027027023</v>
       </c>
       <c r="O9" s="3"/>
       <c r="P9" s="1"/>
@@ -30725,15 +30783,15 @@
     </row>
     <row r="10" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C10" s="3">
-        <v>3</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="D10" s="1">
         <f>2^28/C10</f>
-        <v>89478485.333333328</v>
+        <v>244032232.72727272</v>
       </c>
       <c r="E10" s="2">
         <f>10^9/D10</f>
-        <v>11.175870895385742</v>
+        <v>4.0978193283081055</v>
       </c>
       <c r="O10" s="3"/>
       <c r="P10" s="1"/>
@@ -30741,15 +30799,15 @@
     </row>
     <row r="11" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C11" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D11" s="1">
         <f>2^28/C11</f>
-        <v>53687091.200000003</v>
+        <v>134217728</v>
       </c>
       <c r="E11" s="2">
         <f>10^9/D11</f>
-        <v>18.62645149230957</v>
+        <v>7.4505805969238281</v>
       </c>
       <c r="O11" s="3"/>
       <c r="P11" s="1"/>
@@ -30850,10 +30908,10 @@
       <c r="J14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L14" t="s">
+      <c r="L14" s="2" t="s">
         <v>1</v>
       </c>
       <c r="O14" s="1">
@@ -30880,10 +30938,10 @@
       <c r="V14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="W14" t="s">
+      <c r="W14" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="X14" t="s">
+      <c r="X14" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -30912,10 +30970,10 @@
       <c r="J15" s="2">
         <v>0.13930500000000001</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L15" t="s">
+      <c r="L15" s="2" t="s">
         <v>1</v>
       </c>
       <c r="O15" s="1">
@@ -30942,10 +31000,10 @@
       <c r="V15" s="2">
         <v>0.173397</v>
       </c>
-      <c r="W15" t="s">
+      <c r="W15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="X15" t="s">
+      <c r="X15" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -30974,10 +31032,10 @@
       <c r="J16" s="2">
         <v>0.16684099999999999</v>
       </c>
-      <c r="K16">
+      <c r="K16" s="2">
         <v>0.13677400000000001</v>
       </c>
-      <c r="L16" t="s">
+      <c r="L16" s="2" t="s">
         <v>1</v>
       </c>
       <c r="O16" s="1">
@@ -31004,14 +31062,14 @@
       <c r="V16" s="2">
         <v>0.15396899999999999</v>
       </c>
-      <c r="W16">
+      <c r="W16" s="2">
         <v>0.16625899999999999</v>
       </c>
-      <c r="X16" t="s">
+      <c r="X16" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C17" s="1">
         <v>8192</v>
       </c>
@@ -31036,10 +31094,10 @@
       <c r="J17" s="2">
         <v>0.118898</v>
       </c>
-      <c r="K17">
+      <c r="K17" s="2">
         <v>0.16681499999999999</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="2">
         <v>0.139873</v>
       </c>
       <c r="O17" s="1">
@@ -31066,14 +31124,14 @@
       <c r="V17" s="2">
         <v>0.12113500000000001</v>
       </c>
-      <c r="W17">
+      <c r="W17" s="2">
         <v>0.15184600000000001</v>
       </c>
-      <c r="X17">
+      <c r="X17" s="2">
         <v>0.15746599999999999</v>
       </c>
     </row>
-    <row r="18" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C18" s="1">
         <v>16384</v>
       </c>
@@ -31098,10 +31156,10 @@
       <c r="J18" s="2">
         <v>0.104222</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="2">
         <v>0.12015000000000001</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="2">
         <v>0.16719899999999999</v>
       </c>
       <c r="O18" s="1">
@@ -31128,14 +31186,14 @@
       <c r="V18" s="2">
         <v>0.119377</v>
       </c>
-      <c r="W18">
+      <c r="W18" s="2">
         <v>0.121152</v>
       </c>
-      <c r="X18">
+      <c r="X18" s="2">
         <v>0.15412500000000001</v>
       </c>
     </row>
-    <row r="19" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C19" s="1">
         <v>32768</v>
       </c>
@@ -31160,10 +31218,10 @@
       <c r="J19" s="2">
         <v>0.10177700000000001</v>
       </c>
-      <c r="K19">
+      <c r="K19" s="2">
         <v>0.105255</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="2">
         <v>0.11604</v>
       </c>
       <c r="O19" s="1">
@@ -31190,14 +31248,14 @@
       <c r="V19" s="2">
         <v>0.117691</v>
       </c>
-      <c r="W19">
+      <c r="W19" s="2">
         <v>0.122335</v>
       </c>
-      <c r="X19">
+      <c r="X19" s="2">
         <v>0.121985</v>
       </c>
     </row>
-    <row r="20" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C20" s="1">
         <v>65536</v>
       </c>
@@ -31222,10 +31280,10 @@
       <c r="J20" s="2">
         <v>0.179782</v>
       </c>
-      <c r="K20">
+      <c r="K20" s="2">
         <v>0.11700199999999999</v>
       </c>
-      <c r="L20">
+      <c r="L20" s="2">
         <v>0.12773699999999999</v>
       </c>
       <c r="O20" s="1">
@@ -31252,14 +31310,14 @@
       <c r="V20" s="2">
         <v>0.189721</v>
       </c>
-      <c r="W20">
+      <c r="W20" s="2">
         <v>0.128829</v>
       </c>
-      <c r="X20">
+      <c r="X20" s="2">
         <v>0.124027</v>
       </c>
     </row>
-    <row r="21" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C21" s="1">
         <v>131072</v>
       </c>
@@ -31284,10 +31342,10 @@
       <c r="J21" s="2">
         <v>0.18956799999999999</v>
       </c>
-      <c r="K21">
+      <c r="K21" s="2">
         <v>0.22082599999999999</v>
       </c>
-      <c r="L21">
+      <c r="L21" s="2">
         <v>0.20807600000000001</v>
       </c>
       <c r="O21" s="1">
@@ -31314,14 +31372,14 @@
       <c r="V21" s="2">
         <v>0.19429099999999999</v>
       </c>
-      <c r="W21">
+      <c r="W21" s="2">
         <v>0.22240099999999999</v>
       </c>
-      <c r="X21">
+      <c r="X21" s="2">
         <v>0.20290900000000001</v>
       </c>
     </row>
-    <row r="22" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C22" s="1">
         <v>262144</v>
       </c>
@@ -31346,10 +31404,10 @@
       <c r="J22" s="2">
         <v>0.192194</v>
       </c>
-      <c r="K22">
+      <c r="K22" s="2">
         <v>0.221882</v>
       </c>
-      <c r="L22">
+      <c r="L22" s="2">
         <v>0.29319200000000001</v>
       </c>
       <c r="O22" s="1">
@@ -31376,14 +31434,14 @@
       <c r="V22" s="2">
         <v>0.19595599999999999</v>
       </c>
-      <c r="W22">
+      <c r="W22" s="2">
         <v>0.224354</v>
       </c>
-      <c r="X22">
+      <c r="X22" s="2">
         <v>0.29484900000000003</v>
       </c>
     </row>
-    <row r="23" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C23" s="1">
         <v>524288</v>
       </c>
@@ -31408,10 +31466,10 @@
       <c r="J23" s="2">
         <v>0.37658599999999998</v>
       </c>
-      <c r="K23">
+      <c r="K23" s="2">
         <v>0.38223200000000002</v>
       </c>
-      <c r="L23">
+      <c r="L23" s="2">
         <v>0.38553599999999999</v>
       </c>
       <c r="O23" s="1">
@@ -31438,568 +31496,571 @@
       <c r="V23" s="2">
         <v>0.379187</v>
       </c>
-      <c r="W23">
+      <c r="W23" s="2">
         <v>0.37867099999999998</v>
       </c>
-      <c r="X23">
+      <c r="X23" s="2">
         <v>0.38291199999999997</v>
       </c>
     </row>
-    <row r="24" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C24" s="1">
         <v>1048576</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="2">
         <v>2.5017000000000001E-2</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="2">
         <v>0.116799</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="2">
         <v>0.361761</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="2">
         <v>0.43349799999999999</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="2">
         <v>0.43933899999999998</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="2">
         <v>0.38187399999999999</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="2">
         <v>0.383658</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="2">
         <v>0.38041900000000001</v>
       </c>
-      <c r="L24">
+      <c r="L24" s="2">
         <v>0.38958500000000001</v>
       </c>
       <c r="O24" s="1">
         <v>1048576</v>
       </c>
-      <c r="P24">
+      <c r="P24" s="2">
         <v>0.13214400000000001</v>
       </c>
-      <c r="Q24">
+      <c r="Q24" s="2">
         <v>0.140038</v>
       </c>
-      <c r="R24">
+      <c r="R24" s="2">
         <v>0.35921199999999998</v>
       </c>
-      <c r="S24">
+      <c r="S24" s="2">
         <v>0.42436499999999999</v>
       </c>
-      <c r="T24">
+      <c r="T24" s="2">
         <v>0.434498</v>
       </c>
-      <c r="U24">
+      <c r="U24" s="2">
         <v>0.377216</v>
       </c>
-      <c r="V24">
+      <c r="V24" s="2">
         <v>0.377438</v>
       </c>
-      <c r="W24">
+      <c r="W24" s="2">
         <v>0.38563799999999998</v>
       </c>
-      <c r="X24">
+      <c r="X24" s="2">
         <v>0.38427499999999998</v>
       </c>
     </row>
-    <row r="25" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C25" s="1">
         <v>2097152</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="2">
         <v>2.5201999999999999E-2</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="2">
         <v>0.121452</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="2">
         <v>0.36088799999999999</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="2">
         <v>0.42451100000000003</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="2">
         <v>0.451376</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="2">
         <v>0.38589000000000001</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="2">
         <v>0.37719999999999998</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="2">
         <v>0.386158</v>
       </c>
-      <c r="L25">
+      <c r="L25" s="2">
         <v>0.39099600000000001</v>
       </c>
       <c r="O25" s="1">
         <v>2097152</v>
       </c>
-      <c r="P25">
+      <c r="P25" s="2">
         <v>0.13305600000000001</v>
       </c>
-      <c r="Q25">
+      <c r="Q25" s="2">
         <v>0.141737</v>
       </c>
-      <c r="R25">
+      <c r="R25" s="2">
         <v>0.35838300000000001</v>
       </c>
-      <c r="S25">
+      <c r="S25" s="2">
         <v>0.42604900000000001</v>
       </c>
-      <c r="T25">
+      <c r="T25" s="2">
         <v>0.44006400000000001</v>
       </c>
-      <c r="U25">
+      <c r="U25" s="2">
         <v>0.38098599999999999</v>
       </c>
-      <c r="V25">
+      <c r="V25" s="2">
         <v>0.380019</v>
       </c>
-      <c r="W25">
+      <c r="W25" s="2">
         <v>0.38852900000000001</v>
       </c>
-      <c r="X25">
+      <c r="X25" s="2">
         <v>0.38795400000000002</v>
       </c>
     </row>
-    <row r="26" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C26" s="1">
         <v>4194304</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="2">
         <v>2.6096999999999999E-2</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="2">
         <v>0.13021199999999999</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="2">
         <v>0.38137100000000002</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="2">
         <v>0.46498</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="2">
         <v>0.49726500000000001</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="2">
         <v>0.44257999999999997</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="2">
         <v>0.46590199999999998</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="2">
         <v>0.53358099999999997</v>
       </c>
-      <c r="L26">
+      <c r="L26" s="2">
         <v>0.55742599999999998</v>
       </c>
       <c r="O26" s="1">
         <v>4194304</v>
       </c>
-      <c r="P26">
+      <c r="P26" s="2">
         <v>0.14038100000000001</v>
       </c>
-      <c r="Q26">
+      <c r="Q26" s="2">
         <v>0.157697</v>
       </c>
-      <c r="R26">
+      <c r="R26" s="2">
         <v>0.37626100000000001</v>
       </c>
-      <c r="S26">
+      <c r="S26" s="2">
         <v>0.45872400000000002</v>
       </c>
-      <c r="T26">
+      <c r="T26" s="2">
         <v>0.49197999999999997</v>
       </c>
-      <c r="U26">
+      <c r="U26" s="2">
         <v>0.44505899999999998</v>
       </c>
-      <c r="V26">
+      <c r="V26" s="2">
         <v>0.48186499999999999</v>
       </c>
-      <c r="W26">
+      <c r="W26" s="2">
         <v>0.52334999999999998</v>
       </c>
-      <c r="X26">
+      <c r="X26" s="2">
         <v>0.58506999999999998</v>
       </c>
     </row>
-    <row r="27" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
       <c r="C27" s="1">
         <v>8388608</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="2">
         <v>3.4433999999999999E-2</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="2">
         <v>0.16921800000000001</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="2">
         <v>0.51552699999999996</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="2">
         <v>0.72057400000000005</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="2">
         <v>0.73631000000000002</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="2">
         <v>0.65790899999999997</v>
       </c>
-      <c r="J27">
+      <c r="J27" s="2">
         <v>0.68644700000000003</v>
       </c>
-      <c r="K27">
+      <c r="K27" s="2">
         <v>0.91904300000000005</v>
       </c>
-      <c r="L27">
+      <c r="L27" s="2">
         <v>1.8124910000000001</v>
       </c>
       <c r="O27" s="1">
         <v>8388608</v>
       </c>
-      <c r="P27">
+      <c r="P27" s="2">
         <v>0.13646800000000001</v>
       </c>
-      <c r="Q27">
+      <c r="Q27" s="2">
         <v>0.17319899999999999</v>
       </c>
-      <c r="R27">
+      <c r="R27" s="2">
         <v>0.50101499999999999</v>
       </c>
-      <c r="S27">
+      <c r="S27" s="2">
         <v>0.66889600000000005</v>
       </c>
-      <c r="T27">
+      <c r="T27" s="2">
         <v>0.73406899999999997</v>
       </c>
-      <c r="U27">
+      <c r="U27" s="2">
         <v>0.657744</v>
       </c>
-      <c r="V27">
+      <c r="V27" s="2">
         <v>0.66620100000000004</v>
       </c>
-      <c r="W27">
+      <c r="W27" s="2">
         <v>0.91697799999999996</v>
       </c>
-      <c r="X27">
+      <c r="X27" s="2">
         <v>1.899176</v>
       </c>
     </row>
-    <row r="28" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C28" s="1">
         <v>16777216</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="2">
         <v>4.7648000000000003E-2</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="2">
         <v>0.206788</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="2">
         <v>0.71517500000000001</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="2">
         <v>0.968669</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="2">
         <v>1.0328809999999999</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="2">
         <v>0.95035599999999998</v>
       </c>
-      <c r="J28">
+      <c r="J28" s="2">
         <v>0.92892600000000003</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="2">
         <v>0.95471399999999995</v>
       </c>
-      <c r="L28">
+      <c r="L28" s="2">
         <v>1.7863530000000001</v>
       </c>
       <c r="O28" s="1">
         <v>16777216</v>
       </c>
-      <c r="P28">
+      <c r="P28" s="2">
         <v>0.14415</v>
       </c>
-      <c r="Q28">
+      <c r="Q28" s="2">
         <v>0.20987900000000001</v>
       </c>
-      <c r="R28">
+      <c r="R28" s="2">
         <v>0.70927200000000001</v>
       </c>
-      <c r="S28">
+      <c r="S28" s="2">
         <v>0.93852599999999997</v>
       </c>
-      <c r="T28">
+      <c r="T28" s="2">
         <v>1.0193099999999999</v>
       </c>
-      <c r="U28">
+      <c r="U28" s="2">
         <v>0.92188499999999995</v>
       </c>
-      <c r="V28">
+      <c r="V28" s="2">
         <v>0.91894500000000001</v>
       </c>
-      <c r="W28">
+      <c r="W28" s="2">
         <v>0.93830199999999997</v>
       </c>
-      <c r="X28">
+      <c r="X28" s="2">
         <v>1.7875209999999999</v>
       </c>
     </row>
-    <row r="29" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C29" s="1">
         <v>33554432</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="2">
         <v>5.3926000000000002E-2</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="2">
         <v>0.21967999999999999</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="2">
         <v>0.77917800000000004</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="2">
         <v>1.1142559999999999</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="2">
         <v>1.2128270000000001</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="2">
         <v>1.0979890000000001</v>
       </c>
-      <c r="J29">
+      <c r="J29" s="2">
         <v>1.107888</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="2">
         <v>1.1315539999999999</v>
       </c>
-      <c r="L29">
+      <c r="L29" s="2">
         <v>1.8468059999999999</v>
       </c>
       <c r="O29" s="1">
         <v>33554432</v>
       </c>
-      <c r="P29">
+      <c r="P29" s="2">
         <v>0.14243</v>
       </c>
-      <c r="Q29">
+      <c r="Q29" s="2">
         <v>0.22158700000000001</v>
       </c>
-      <c r="R29">
+      <c r="R29" s="2">
         <v>0.78307199999999999</v>
       </c>
-      <c r="S29">
+      <c r="S29" s="2">
         <v>1.0883020000000001</v>
       </c>
-      <c r="T29">
+      <c r="T29" s="2">
         <v>1.2228429999999999</v>
       </c>
-      <c r="U29">
+      <c r="U29" s="2">
         <v>1.0821419999999999</v>
       </c>
-      <c r="V29">
+      <c r="V29" s="2">
         <v>1.109518</v>
       </c>
-      <c r="W29">
+      <c r="W29" s="2">
         <v>1.1239269999999999</v>
       </c>
-      <c r="X29">
+      <c r="X29" s="2">
         <v>1.8344309999999999</v>
       </c>
     </row>
-    <row r="30" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C30" s="1">
         <v>67108864</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="2">
         <v>5.6356000000000003E-2</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="2">
         <v>0.22332399999999999</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="2">
         <v>0.81923800000000002</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="2">
         <v>1.1763300000000001</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="2">
         <v>1.2693030000000001</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="2">
         <v>1.157942</v>
       </c>
-      <c r="J30">
+      <c r="J30" s="2">
         <v>1.1636679999999999</v>
       </c>
-      <c r="K30">
+      <c r="K30" s="2">
         <v>1.2256229999999999</v>
       </c>
-      <c r="L30">
+      <c r="L30" s="2">
         <v>1.839604</v>
       </c>
       <c r="O30" s="1">
         <v>67108864</v>
       </c>
-      <c r="P30">
+      <c r="P30" s="2">
         <v>0.144763</v>
       </c>
-      <c r="Q30">
+      <c r="Q30" s="2">
         <v>0.227932</v>
       </c>
-      <c r="R30">
+      <c r="R30" s="2">
         <v>0.804257</v>
       </c>
-      <c r="S30">
+      <c r="S30" s="2">
         <v>1.1450819999999999</v>
       </c>
-      <c r="T30">
+      <c r="T30" s="2">
         <v>1.2818849999999999</v>
       </c>
-      <c r="U30">
+      <c r="U30" s="2">
         <v>1.1663239999999999</v>
       </c>
-      <c r="V30">
+      <c r="V30" s="2">
         <v>1.1638470000000001</v>
       </c>
-      <c r="W30">
+      <c r="W30" s="2">
         <v>1.1778649999999999</v>
       </c>
-      <c r="X30">
+      <c r="X30" s="2">
         <v>1.820878</v>
       </c>
     </row>
-    <row r="31" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C31" s="1">
         <v>134217728</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="2">
         <v>7.0610000000000006E-2</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="2">
         <v>0.25789400000000001</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="2">
         <v>0.90912999999999999</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="2">
         <v>1.29175</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="2">
         <v>1.4200440000000001</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="2">
         <v>1.3849089999999999</v>
       </c>
-      <c r="J31">
+      <c r="J31" s="2">
         <v>1.396841</v>
       </c>
-      <c r="K31">
+      <c r="K31" s="2">
         <v>1.4889349999999999</v>
       </c>
-      <c r="L31">
+      <c r="L31" s="2">
         <v>2.1339830000000002</v>
       </c>
       <c r="O31" s="1">
         <v>134217728</v>
       </c>
-      <c r="P31">
+      <c r="P31" s="2">
         <v>0.14199999999999999</v>
       </c>
-      <c r="Q31">
+      <c r="Q31" s="2">
         <v>0.26524999999999999</v>
       </c>
-      <c r="R31">
+      <c r="R31" s="2">
         <v>0.91329700000000003</v>
       </c>
-      <c r="S31">
+      <c r="S31" s="2">
         <v>1.2915989999999999</v>
       </c>
-      <c r="T31">
+      <c r="T31" s="2">
         <v>1.41615</v>
       </c>
-      <c r="U31">
+      <c r="U31" s="2">
         <v>1.3512980000000001</v>
       </c>
-      <c r="V31">
+      <c r="V31" s="2">
         <v>1.403705</v>
       </c>
-      <c r="W31">
+      <c r="W31" s="2">
         <v>1.5575000000000001</v>
       </c>
-      <c r="X31">
+      <c r="X31" s="2">
         <v>2.019412</v>
       </c>
     </row>
-    <row r="32" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C32" s="1">
         <v>268435456</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="2">
         <v>7.3663999999999993E-2</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="2">
         <v>0.30150300000000002</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="2">
         <v>1.101567</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="2">
         <v>1.634468</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="2">
         <v>1.736029</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="2">
         <v>1.724348</v>
       </c>
-      <c r="J32">
+      <c r="J32" s="2">
         <v>1.914712</v>
       </c>
-      <c r="K32">
+      <c r="K32" s="2">
         <v>1.945319</v>
       </c>
-      <c r="L32">
+      <c r="L32" s="2">
         <v>2.4180990000000002</v>
       </c>
       <c r="O32" s="1">
         <v>268435456</v>
       </c>
-      <c r="P32">
+      <c r="P32" s="2">
         <v>0.15577099999999999</v>
       </c>
-      <c r="Q32">
+      <c r="Q32" s="2">
         <v>0.30995200000000001</v>
       </c>
-      <c r="R32">
+      <c r="R32" s="2">
         <v>1.1263840000000001</v>
       </c>
-      <c r="S32">
+      <c r="S32" s="2">
         <v>1.6532230000000001</v>
       </c>
-      <c r="T32">
+      <c r="T32" s="2">
         <v>1.6704969999999999</v>
       </c>
-      <c r="U32">
+      <c r="U32" s="2">
         <v>1.604136</v>
       </c>
-      <c r="V32">
+      <c r="V32" s="2">
         <v>1.729077</v>
       </c>
-      <c r="W32">
+      <c r="W32" s="2">
         <v>1.848231</v>
       </c>
-      <c r="X32">
+      <c r="X32" s="2">
         <v>2.2939970000000001</v>
       </c>
     </row>
@@ -32007,61 +32068,61 @@
       <c r="C33" s="1">
         <v>536870912</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="2">
         <v>7.2221999999999995E-2</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="2">
         <v>0.301344</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="2">
         <v>1.251044</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="2">
         <v>1.6606959999999999</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="2">
         <v>1.9342950000000001</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="2">
         <v>1.819809</v>
       </c>
-      <c r="J33">
+      <c r="J33" s="2">
         <v>1.920974</v>
       </c>
-      <c r="K33">
+      <c r="K33" s="2">
         <v>2.0746859999999998</v>
       </c>
-      <c r="L33">
+      <c r="L33" s="2">
         <v>2.447778</v>
       </c>
       <c r="O33" s="1">
         <v>536870912</v>
       </c>
-      <c r="P33">
+      <c r="P33" s="2">
         <v>0.152559</v>
       </c>
-      <c r="Q33">
+      <c r="Q33" s="2">
         <v>0.30471199999999998</v>
       </c>
-      <c r="R33">
+      <c r="R33" s="2">
         <v>1.0934269999999999</v>
       </c>
-      <c r="S33">
+      <c r="S33" s="2">
         <v>1.5983719999999999</v>
       </c>
-      <c r="T33">
+      <c r="T33" s="2">
         <v>1.9011640000000001</v>
       </c>
-      <c r="U33">
+      <c r="U33" s="2">
         <v>1.794411</v>
       </c>
-      <c r="V33">
+      <c r="V33" s="2">
         <v>1.9121269999999999</v>
       </c>
-      <c r="W33">
+      <c r="W33" s="2">
         <v>2.0576539999999999</v>
       </c>
-      <c r="X33">
+      <c r="X33" s="2">
         <v>2.4898020000000001</v>
       </c>
     </row>
@@ -32069,63 +32130,83 @@
       <c r="C34" s="1">
         <v>1073741824</v>
       </c>
-      <c r="D34">
+      <c r="D34" s="2">
         <v>7.0574999999999999E-2</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="2">
         <v>0.296462</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="2">
         <v>1.1014969999999999</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="2">
         <v>1.633999</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="2">
         <v>1.971106</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="2">
         <v>1.803272</v>
       </c>
-      <c r="J34">
+      <c r="J34" s="2">
         <v>1.9602550000000001</v>
       </c>
-      <c r="K34">
+      <c r="K34" s="2">
         <v>2.1334499999999998</v>
       </c>
-      <c r="L34">
+      <c r="L34" s="2">
         <v>2.599237</v>
       </c>
       <c r="O34" s="1">
         <v>1073741824</v>
       </c>
-      <c r="P34">
+      <c r="P34" s="2">
         <v>0.149529</v>
       </c>
-      <c r="Q34">
+      <c r="Q34" s="2">
         <v>0.29759099999999999</v>
       </c>
-      <c r="R34">
+      <c r="R34" s="2">
         <v>1.127624</v>
       </c>
-      <c r="S34">
+      <c r="S34" s="2">
         <v>1.6495610000000001</v>
       </c>
-      <c r="T34">
+      <c r="T34" s="2">
         <v>1.997838</v>
       </c>
-      <c r="U34">
+      <c r="U34" s="2">
         <v>1.8553649999999999</v>
       </c>
-      <c r="V34">
+      <c r="V34" s="2">
         <v>1.9874510000000001</v>
       </c>
-      <c r="W34">
+      <c r="W34" s="2">
         <v>2.1927599999999998</v>
       </c>
-      <c r="X34">
+      <c r="X34" s="2">
         <v>2.4894910000000001</v>
       </c>
+    </row>
+    <row r="35" spans="3:24" x14ac:dyDescent="0.2">
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="2"/>
+      <c r="L35" s="2"/>
+      <c r="P35" s="2"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="2"/>
+      <c r="W35" s="2"/>
+      <c r="X35" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -32139,10 +32220,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="C1:X33"/>
+  <dimension ref="B1:X33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36:X76"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -32189,20 +32270,32 @@
       <c r="E6" t="s">
         <v>8</v>
       </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
       <c r="O6"/>
     </row>
     <row r="7" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C7" s="3">
-        <f>0.01</f>
-        <v>0.01</v>
+        <v>0.6</v>
       </c>
       <c r="D7" s="1">
         <f>2^28/C7</f>
-        <v>26843545600</v>
+        <v>447392426.66666669</v>
       </c>
       <c r="E7" s="2">
         <f>10^9/D7</f>
-        <v>3.7252902984619141E-2</v>
+        <v>2.2351741790771484</v>
+      </c>
+      <c r="F7" s="5">
+        <f>E7/$I$8</f>
+        <v>3.3527612686157227</v>
+      </c>
+      <c r="H7" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" t="s">
+        <v>12</v>
       </c>
       <c r="O7" s="3"/>
       <c r="P7" s="1"/>
@@ -32210,15 +32303,26 @@
     </row>
     <row r="8" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C8" s="3">
-        <v>0.1</v>
+        <v>2.7</v>
       </c>
       <c r="D8" s="1">
         <f>2^28/C8</f>
-        <v>2684354560</v>
+        <v>99420539.259259254</v>
       </c>
       <c r="E8" s="2">
         <f>10^9/D8</f>
-        <v>0.37252902984619141</v>
+        <v>10.058283805847168</v>
+      </c>
+      <c r="F8" s="5">
+        <f>E8/$I$8</f>
+        <v>15.087425708770752</v>
+      </c>
+      <c r="H8">
+        <v>1.5</v>
+      </c>
+      <c r="I8" s="4">
+        <f>1/H8</f>
+        <v>0.66666666666666663</v>
       </c>
       <c r="O8" s="3"/>
       <c r="P8" s="1"/>
@@ -32226,15 +32330,19 @@
     </row>
     <row r="9" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C9" s="3">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D9" s="1">
         <f>2^28/C9</f>
-        <v>268435456</v>
+        <v>26843545.600000001</v>
       </c>
       <c r="E9" s="2">
         <f>10^9/D9</f>
-        <v>3.7252902984619141</v>
+        <v>37.252902984619141</v>
+      </c>
+      <c r="F9" s="5">
+        <f>E9/$I$8</f>
+        <v>55.879354476928711</v>
       </c>
       <c r="O9" s="3"/>
       <c r="P9" s="1"/>
@@ -32242,15 +32350,19 @@
     </row>
     <row r="10" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C10" s="3">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="D10" s="1">
         <f>2^28/C10</f>
-        <v>89478485.333333328</v>
+        <v>10737418.24</v>
       </c>
       <c r="E10" s="2">
         <f>10^9/D10</f>
-        <v>11.175870895385742</v>
+        <v>93.132257461547852</v>
+      </c>
+      <c r="F10" s="5">
+        <f>E10/$I$8</f>
+        <v>139.69838619232178</v>
       </c>
       <c r="O10" s="3"/>
       <c r="P10" s="1"/>
@@ -32258,15 +32370,19 @@
     </row>
     <row r="11" spans="3:24" x14ac:dyDescent="0.2">
       <c r="C11" s="3">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="D11" s="1">
         <f>2^28/C11</f>
-        <v>53687091.200000003</v>
+        <v>5368709.1200000001</v>
       </c>
       <c r="E11" s="2">
         <f>10^9/D11</f>
-        <v>18.62645149230957</v>
+        <v>186.2645149230957</v>
+      </c>
+      <c r="F11" s="5">
+        <f>E11/$I$8</f>
+        <v>279.39677238464355</v>
       </c>
       <c r="O11" s="3"/>
       <c r="P11" s="1"/>
@@ -32528,7 +32644,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C17" s="1">
         <v>8192</v>
       </c>
@@ -32590,7 +32706,7 @@
         <v>1.8335840000000001</v>
       </c>
     </row>
-    <row r="18" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C18" s="1">
         <v>16384</v>
       </c>
@@ -32652,7 +32768,7 @@
         <v>1.0111749999999999</v>
       </c>
     </row>
-    <row r="19" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C19" s="1">
         <v>32768</v>
       </c>
@@ -32714,7 +32830,10 @@
         <v>0.80701400000000001</v>
       </c>
     </row>
-    <row r="20" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>15</v>
+      </c>
       <c r="C20" s="1">
         <v>65536</v>
       </c>
@@ -32776,7 +32895,7 @@
         <v>1.091134</v>
       </c>
     </row>
-    <row r="21" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C21" s="1">
         <v>131072</v>
       </c>
@@ -32838,7 +32957,7 @@
         <v>1.0724549999999999</v>
       </c>
     </row>
-    <row r="22" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C22" s="1">
         <v>262144</v>
       </c>
@@ -32900,7 +33019,10 @@
         <v>0.95737499999999998</v>
       </c>
     </row>
-    <row r="23" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
       <c r="C23" s="1">
         <v>524288</v>
       </c>
@@ -32962,7 +33084,7 @@
         <v>1.025569</v>
       </c>
     </row>
-    <row r="24" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C24" s="1">
         <v>1048576</v>
       </c>
@@ -33024,7 +33146,7 @@
         <v>33.502597999999999</v>
       </c>
     </row>
-    <row r="25" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C25" s="1">
         <v>2097152</v>
       </c>
@@ -33086,7 +33208,7 @@
         <v>39.637282999999996</v>
       </c>
     </row>
-    <row r="26" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C26" s="1">
         <v>4194304</v>
       </c>
@@ -33148,7 +33270,7 @@
         <v>40.815773999999998</v>
       </c>
     </row>
-    <row r="27" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C27" s="1">
         <v>8388608</v>
       </c>
@@ -33207,7 +33329,7 @@
         <v>40.301859</v>
       </c>
     </row>
-    <row r="28" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C28" s="1">
         <v>16777216</v>
       </c>
@@ -33269,7 +33391,7 @@
         <v>40.542597999999998</v>
       </c>
     </row>
-    <row r="29" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C29" s="1">
         <v>33554432</v>
       </c>
@@ -33331,7 +33453,7 @@
         <v>42.727296000000003</v>
       </c>
     </row>
-    <row r="30" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C30" s="1">
         <v>67108864</v>
       </c>
@@ -33393,7 +33515,7 @@
         <v>65.775902000000002</v>
       </c>
     </row>
-    <row r="31" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C31" s="1">
         <v>134217728</v>
       </c>
@@ -33455,7 +33577,7 @@
         <v>70.491669000000002</v>
       </c>
     </row>
-    <row r="32" spans="3:24" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:24" x14ac:dyDescent="0.2">
       <c r="C32" s="1">
         <v>268435456</v>
       </c>

</xml_diff>